<commit_message>
implemented prop calculations method to perform calculations; goal: finding solution for putting information into rows
</commit_message>
<xml_diff>
--- a/Order Template/Order 2_FaceTalk_Uzbek.xlsx
+++ b/Order Template/Order 2_FaceTalk_Uzbek.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dharjianto/Documents/Projects/order-analysis/Order Template/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7B7D1EF-2F45-7D4E-9BDD-A703943B2236}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CB9457A-BBEC-D44E-8D9B-E0C18D99FDDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -623,14 +623,6 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -642,6 +634,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1001,7 +1001,7 @@
   <dimension ref="A1:R79"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="92" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1029,18 +1029,18 @@
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="B2" s="29" t="s">
+      <c r="B2" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
-      <c r="F2" s="30"/>
-      <c r="G2" s="30"/>
-      <c r="H2" s="30"/>
-      <c r="I2" s="30"/>
-      <c r="J2" s="30"/>
-      <c r="K2" s="30"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="26"/>
+      <c r="G2" s="26"/>
+      <c r="H2" s="26"/>
+      <c r="I2" s="26"/>
+      <c r="J2" s="26"/>
+      <c r="K2" s="26"/>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B3" s="2"/>
@@ -1087,14 +1087,8 @@
       <c r="B5" s="22"/>
       <c r="C5" s="22"/>
       <c r="D5" s="22"/>
-      <c r="E5" s="21" t="e">
-        <f>C5/(C5+D5)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F5" s="21" t="e">
-        <f>D5/(C5+D5)</f>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="E5" s="21"/>
+      <c r="F5" s="21"/>
       <c r="G5" s="21"/>
       <c r="H5" s="21" t="s">
         <v>13</v>
@@ -1102,13 +1096,13 @@
       <c r="K5" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="L5" s="21" t="e">
+      <c r="L5" s="21">
         <f t="shared" ref="L5:M7" si="0">E5</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M5" s="21" t="e">
+        <v>0</v>
+      </c>
+      <c r="M5" s="21">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:18" ht="19" customHeight="1" x14ac:dyDescent="0.25">
@@ -1118,14 +1112,8 @@
       <c r="B6" s="22"/>
       <c r="C6" s="22"/>
       <c r="D6" s="22"/>
-      <c r="E6" s="21" t="e">
-        <f>C6/(C6+D6)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F6" s="21" t="e">
-        <f>D6/(C6+D6)</f>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="E6" s="21"/>
+      <c r="F6" s="21"/>
       <c r="G6" s="21"/>
       <c r="H6" s="21" t="s">
         <v>14</v>
@@ -1133,13 +1121,13 @@
       <c r="K6" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="L6" s="21" t="e">
+      <c r="L6" s="21">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M6" s="21" t="e">
+        <v>0</v>
+      </c>
+      <c r="M6" s="21">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:18" ht="19" customHeight="1" x14ac:dyDescent="0.25">
@@ -1149,14 +1137,8 @@
       <c r="B7" s="22"/>
       <c r="C7" s="22"/>
       <c r="D7" s="22"/>
-      <c r="E7" s="21" t="e">
-        <f>C7/(C7+D7)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F7" s="21" t="e">
-        <f>D7/(C7+D7)</f>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="E7" s="21"/>
+      <c r="F7" s="21"/>
       <c r="G7" s="21"/>
       <c r="H7" s="21" t="s">
         <v>15</v>
@@ -1164,13 +1146,13 @@
       <c r="K7" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="L7" s="21" t="e">
+      <c r="L7" s="21">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M7" s="21" t="e">
+        <v>0</v>
+      </c>
+      <c r="M7" s="21">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:18" ht="19" customHeight="1" x14ac:dyDescent="0.25">
@@ -1180,14 +1162,8 @@
       <c r="B8" s="22"/>
       <c r="C8" s="22"/>
       <c r="D8" s="22"/>
-      <c r="E8" s="21" t="e">
-        <f>C8/(C8+D8)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F8" s="21" t="e">
-        <f>D8/(C8+D8)</f>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="E8" s="21"/>
+      <c r="F8" s="21"/>
       <c r="G8" s="21"/>
       <c r="H8" s="8" t="s">
         <v>16</v>
@@ -1195,13 +1171,13 @@
       <c r="K8" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="L8" s="17" t="e">
+      <c r="L8" s="17">
         <f>AVERAGE(L5:L7)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M8" s="17" t="e">
+        <v>0</v>
+      </c>
+      <c r="M8" s="17">
         <f>AVERAGE(M5:M7)</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:18" ht="19" customHeight="1" x14ac:dyDescent="0.25">
@@ -1212,10 +1188,7 @@
       <c r="C9" s="22"/>
       <c r="D9" s="22"/>
       <c r="F9" s="21"/>
-      <c r="G9" s="21">
-        <f>B9</f>
-        <v>0</v>
-      </c>
+      <c r="G9" s="21"/>
       <c r="H9" s="16" t="s">
         <v>18</v>
       </c>
@@ -1248,14 +1221,8 @@
       <c r="B10" s="22"/>
       <c r="C10" s="22"/>
       <c r="D10" s="22"/>
-      <c r="E10" s="21" t="e">
-        <f>C10/(C10+D10)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F10" s="21" t="e">
-        <f>D10/(C10+D10)</f>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="E10" s="21"/>
+      <c r="F10" s="21"/>
       <c r="G10" s="21"/>
       <c r="H10" s="8" t="s">
         <v>24</v>
@@ -1263,28 +1230,28 @@
       <c r="K10" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="L10" s="21" t="e">
+      <c r="L10" s="21">
         <f>E11</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M10" s="21" t="e">
+        <v>0</v>
+      </c>
+      <c r="M10" s="21">
         <f>F11</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N10" t="e">
+        <v>0</v>
+      </c>
+      <c r="N10">
         <f>M10</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="P10" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="Q10" s="21" t="e">
+      <c r="Q10" s="21">
         <f>F13</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="R10" s="21" t="e">
+        <v>0</v>
+      </c>
+      <c r="R10" s="21">
         <f>Q10-M10</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:18" ht="19" customHeight="1" x14ac:dyDescent="0.25">
@@ -1294,14 +1261,8 @@
       <c r="B11" s="22"/>
       <c r="C11" s="22"/>
       <c r="D11" s="22"/>
-      <c r="E11" s="21" t="e">
-        <f>C11/(C11+D11)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F11" s="21" t="e">
-        <f>D11/(C11+D11)</f>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="E11" s="21"/>
+      <c r="F11" s="21"/>
       <c r="G11" s="21"/>
       <c r="H11" s="8" t="s">
         <v>25</v>
@@ -1309,28 +1270,28 @@
       <c r="K11" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="L11" s="21" t="e">
+      <c r="L11" s="21">
         <f>E77</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M11" s="21" t="e">
+        <v>0</v>
+      </c>
+      <c r="M11" s="21">
         <f>F77</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N11" t="e">
+        <v>0</v>
+      </c>
+      <c r="N11">
         <f>L11</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="P11" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="Q11" s="21" t="e">
+      <c r="Q11" s="21">
         <f>E79</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="R11" s="21" t="e">
+        <v>0</v>
+      </c>
+      <c r="R11" s="21">
         <f>Q11-L11</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:18" ht="19" customHeight="1" x14ac:dyDescent="0.25">
@@ -1340,38 +1301,35 @@
       <c r="B12" s="22"/>
       <c r="C12" s="22"/>
       <c r="D12" s="22"/>
-      <c r="G12" s="21">
-        <f>B12</f>
-        <v>0</v>
-      </c>
+      <c r="G12" s="21"/>
       <c r="H12" s="16" t="s">
         <v>29</v>
       </c>
       <c r="K12" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="L12" s="21" t="e">
+      <c r="L12" s="21">
         <f>E41</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M12" s="21" t="e">
+        <v>0</v>
+      </c>
+      <c r="M12" s="21">
         <f>F41</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N12" t="e">
+        <v>0</v>
+      </c>
+      <c r="N12">
         <f>M12</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="P12" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="Q12" s="21" t="e">
+      <c r="Q12" s="21">
         <f>F43</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="R12" s="21" t="e">
+        <v>0</v>
+      </c>
+      <c r="R12" s="21">
         <f>Q12-M12</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:18" ht="19" customHeight="1" x14ac:dyDescent="0.25">
@@ -1381,14 +1339,8 @@
       <c r="B13" s="22"/>
       <c r="C13" s="22"/>
       <c r="D13" s="22"/>
-      <c r="E13" s="21" t="e">
-        <f>C13/(C13+D13)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F13" s="21" t="e">
-        <f>D13/(C13+D13)</f>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="E13" s="21"/>
+      <c r="F13" s="21"/>
       <c r="G13" s="21"/>
       <c r="H13" s="8" t="s">
         <v>26</v>
@@ -1396,28 +1348,28 @@
       <c r="K13" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="L13" s="21" t="e">
+      <c r="L13" s="21">
         <f>E53</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M13" s="21" t="e">
+        <v>0</v>
+      </c>
+      <c r="M13" s="21">
         <f>F53</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N13" t="e">
+        <v>0</v>
+      </c>
+      <c r="N13">
         <f>L13</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="P13" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="Q13" s="21" t="e">
+      <c r="Q13" s="21">
         <f>E55</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="R13" s="21" t="e">
+        <v>0</v>
+      </c>
+      <c r="R13" s="21">
         <f>Q13-L13</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:18" ht="19" customHeight="1" x14ac:dyDescent="0.25">
@@ -1427,14 +1379,8 @@
       <c r="B14" s="22"/>
       <c r="C14" s="22"/>
       <c r="D14" s="22"/>
-      <c r="E14" s="21" t="e">
-        <f>C14/(C14+D14)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F14" s="21" t="e">
-        <f>D14/(C14+D14)</f>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="E14" s="21"/>
+      <c r="F14" s="21"/>
       <c r="G14" s="21"/>
       <c r="H14" s="21" t="s">
         <v>34</v>
@@ -1442,28 +1388,28 @@
       <c r="K14" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="L14" s="21" t="e">
+      <c r="L14" s="21">
         <f>E17</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M14" s="21" t="e">
+        <v>0</v>
+      </c>
+      <c r="M14" s="21">
         <f>F17</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N14" t="e">
+        <v>0</v>
+      </c>
+      <c r="N14">
         <f>M14</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="P14" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="Q14" s="21" t="e">
+      <c r="Q14" s="21">
         <f>F19</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="R14" s="21" t="e">
+        <v>0</v>
+      </c>
+      <c r="R14" s="21">
         <f>Q14-M14</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:18" ht="19" customHeight="1" x14ac:dyDescent="0.25">
@@ -1475,10 +1421,7 @@
       <c r="D15" s="22"/>
       <c r="E15" s="21"/>
       <c r="F15" s="21"/>
-      <c r="G15" s="21">
-        <f>B15</f>
-        <v>0</v>
-      </c>
+      <c r="G15" s="21"/>
       <c r="H15" s="5" t="s">
         <v>37</v>
       </c>
@@ -1490,13 +1433,13 @@
       <c r="P15" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="Q15" s="21" t="e">
+      <c r="Q15" s="21">
         <f>E31</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="R15" s="21" t="e">
+        <v>0</v>
+      </c>
+      <c r="R15" s="21">
         <f>Q15-L15</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:18" ht="19" customHeight="1" x14ac:dyDescent="0.25">
@@ -1506,14 +1449,8 @@
       <c r="B16" s="22"/>
       <c r="C16" s="22"/>
       <c r="D16" s="22"/>
-      <c r="E16" s="21" t="e">
-        <f>C16/(C16+D16)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F16" s="21" t="e">
-        <f>D16/(C16+D16)</f>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="E16" s="21"/>
+      <c r="F16" s="21"/>
       <c r="G16" s="21"/>
       <c r="H16" s="21" t="s">
         <v>40</v>
@@ -1521,28 +1458,28 @@
       <c r="K16" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="L16" s="17" t="e">
+      <c r="L16" s="17">
         <f>AVERAGE(L10:L15)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M16" s="17" t="e">
+        <v>0</v>
+      </c>
+      <c r="M16" s="17">
         <f>AVERAGE(M10:M15)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N16" t="e">
+        <v>0</v>
+      </c>
+      <c r="N16">
         <f>AVERAGE(N10:N15)</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="P16" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="Q16" s="17" t="e">
+      <c r="Q16" s="17">
         <f>AVERAGE(Q10:Q15)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="R16" s="17" t="e">
+        <v>0</v>
+      </c>
+      <c r="R16" s="17">
         <f>AVERAGE(R10:R15)</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:18" ht="19" customHeight="1" x14ac:dyDescent="0.25">
@@ -1552,14 +1489,8 @@
       <c r="B17" s="22"/>
       <c r="C17" s="22"/>
       <c r="D17" s="22"/>
-      <c r="E17" s="21" t="e">
-        <f>C17/(C17+D17)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F17" s="21" t="e">
-        <f>D17/(C17+D17)</f>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="E17" s="21"/>
+      <c r="F17" s="21"/>
       <c r="G17" s="21"/>
       <c r="H17" s="21" t="s">
         <v>35</v>
@@ -1595,38 +1526,35 @@
       <c r="D18" s="22"/>
       <c r="E18" s="21"/>
       <c r="F18" s="21"/>
-      <c r="G18" s="8">
-        <f>B18</f>
-        <v>0</v>
-      </c>
+      <c r="G18" s="8"/>
       <c r="H18" s="5" t="s">
         <v>43</v>
       </c>
       <c r="K18" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="L18" s="21" t="e">
+      <c r="L18" s="21">
         <f>E65</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M18" s="21" t="e">
+        <v>0</v>
+      </c>
+      <c r="M18" s="21">
         <f>F65</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N18" t="e">
+        <v>0</v>
+      </c>
+      <c r="N18">
         <f>M18</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="P18" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="Q18" s="21" t="e">
+      <c r="Q18" s="21">
         <f>F67</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="R18" s="21" t="e">
+        <v>0</v>
+      </c>
+      <c r="R18" s="21">
         <f>Q18-M18</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:18" ht="19" customHeight="1" x14ac:dyDescent="0.25">
@@ -1636,14 +1564,8 @@
       <c r="B19" s="22"/>
       <c r="C19" s="22"/>
       <c r="D19" s="22"/>
-      <c r="E19" s="21" t="e">
-        <f>C19/(C19+D19)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F19" s="21" t="e">
-        <f>D19/(C19+D19)</f>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="E19" s="21"/>
+      <c r="F19" s="21"/>
       <c r="G19" s="21"/>
       <c r="H19" s="8" t="s">
         <v>36</v>
@@ -1656,13 +1578,13 @@
       <c r="P19" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="Q19" s="21" t="e">
+      <c r="Q19" s="21">
         <f>E25</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="R19" s="21" t="e">
+        <v>0</v>
+      </c>
+      <c r="R19" s="21">
         <f>Q19-L19</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:18" ht="19" customHeight="1" x14ac:dyDescent="0.25">
@@ -1672,14 +1594,8 @@
       <c r="B20" s="22"/>
       <c r="C20" s="22"/>
       <c r="D20" s="22"/>
-      <c r="E20" s="21" t="e">
-        <f>C20/(C20+D20)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F20" s="21" t="e">
-        <f>D20/(C20+D20)</f>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="E20" s="21"/>
+      <c r="F20" s="21"/>
       <c r="G20" s="21"/>
       <c r="H20" s="21" t="s">
         <v>48</v>
@@ -1687,28 +1603,28 @@
       <c r="K20" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="L20" s="21" t="e">
+      <c r="L20" s="21">
         <f>E32</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M20" s="21" t="e">
+        <v>0</v>
+      </c>
+      <c r="M20" s="21">
         <f>F32</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N20" t="e">
+        <v>0</v>
+      </c>
+      <c r="N20">
         <f>M20</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="P20" s="21" t="s">
         <v>50</v>
       </c>
-      <c r="Q20" s="21" t="e">
+      <c r="Q20" s="21">
         <f>F34</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="R20" s="21" t="e">
+        <v>0</v>
+      </c>
+      <c r="R20" s="21">
         <f>Q20-M20</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:18" ht="19" customHeight="1" x14ac:dyDescent="0.25">
@@ -1720,38 +1636,35 @@
       <c r="D21" s="22"/>
       <c r="E21" s="21"/>
       <c r="F21" s="21"/>
-      <c r="G21" s="8">
-        <f>B21</f>
-        <v>0</v>
-      </c>
+      <c r="G21" s="8"/>
       <c r="H21" s="5" t="s">
         <v>51</v>
       </c>
       <c r="K21" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="L21" s="21" t="e">
+      <c r="L21" s="21">
         <f>E71</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M21" s="21" t="e">
+        <v>0</v>
+      </c>
+      <c r="M21" s="21">
         <f>F71</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N21" t="e">
+        <v>0</v>
+      </c>
+      <c r="N21">
         <f>L21</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="P21" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="Q21" s="21" t="e">
+      <c r="Q21" s="21">
         <f>E73</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="R21" s="21" t="e">
+        <v>0</v>
+      </c>
+      <c r="R21" s="21">
         <f>Q21-L21</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:18" ht="19" customHeight="1" x14ac:dyDescent="0.25">
@@ -1761,14 +1674,8 @@
       <c r="B22" s="22"/>
       <c r="C22" s="22"/>
       <c r="D22" s="22"/>
-      <c r="E22" s="21" t="e">
-        <f>C22/(C22+D22)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F22" s="21" t="e">
-        <f>D22/(C22+D22)</f>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="E22" s="21"/>
+      <c r="F22" s="21"/>
       <c r="G22" s="21"/>
       <c r="H22" s="8" t="s">
         <v>54</v>
@@ -1776,28 +1683,28 @@
       <c r="K22" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="L22" s="21" t="e">
+      <c r="L22" s="21">
         <f>E59</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M22" s="21" t="e">
+        <v>0</v>
+      </c>
+      <c r="M22" s="21">
         <f>F59</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N22" t="e">
+        <v>0</v>
+      </c>
+      <c r="N22">
         <f>M22</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="P22" s="21" t="s">
         <v>56</v>
       </c>
-      <c r="Q22" s="21" t="e">
+      <c r="Q22" s="21">
         <f>F61</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="R22" s="21" t="e">
+        <v>0</v>
+      </c>
+      <c r="R22" s="21">
         <f>Q22-M22</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:18" ht="19" customHeight="1" x14ac:dyDescent="0.25">
@@ -1807,12 +1714,8 @@
       <c r="B23" s="22"/>
       <c r="C23" s="22"/>
       <c r="D23" s="22"/>
-      <c r="E23" s="21">
-        <v>0</v>
-      </c>
-      <c r="F23" s="21">
-        <v>0</v>
-      </c>
+      <c r="E23" s="21"/>
+      <c r="F23" s="21"/>
       <c r="G23" s="21"/>
       <c r="H23" s="21" t="s">
         <v>46</v>
@@ -1820,28 +1723,28 @@
       <c r="K23" s="21" t="s">
         <v>57</v>
       </c>
-      <c r="L23" s="21" t="e">
+      <c r="L23" s="21">
         <f>E47</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M23" s="21" t="e">
+        <v>0</v>
+      </c>
+      <c r="M23" s="21">
         <f>F47</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N23" t="e">
+        <v>0</v>
+      </c>
+      <c r="N23">
         <f>L23</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="P23" s="21" t="s">
         <v>58</v>
       </c>
-      <c r="Q23" s="21" t="e">
+      <c r="Q23" s="21">
         <f>E49</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="R23" s="21" t="e">
+        <v>0</v>
+      </c>
+      <c r="R23" s="21">
         <f>Q23-L23</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:18" ht="19" customHeight="1" x14ac:dyDescent="0.25">
@@ -1853,38 +1756,35 @@
       <c r="D24" s="22"/>
       <c r="E24" s="21"/>
       <c r="F24" s="21"/>
-      <c r="G24" s="8">
-        <f>B24</f>
-        <v>0</v>
-      </c>
+      <c r="G24" s="8"/>
       <c r="H24" s="5" t="s">
         <v>59</v>
       </c>
       <c r="K24" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="L24" s="17" t="e">
+      <c r="L24" s="17">
         <f>AVERAGE(L18:L23)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M24" s="17" t="e">
+        <v>0</v>
+      </c>
+      <c r="M24" s="17">
         <f>AVERAGE(M18:M23)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N24" t="e">
+        <v>0</v>
+      </c>
+      <c r="N24">
         <f>AVERAGE(N18:N23)</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="P24" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="Q24" s="17" t="e">
+      <c r="Q24" s="17">
         <f>AVERAGE(Q18:Q23)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="R24" s="17" t="e">
+        <v>0</v>
+      </c>
+      <c r="R24" s="17">
         <f>AVERAGE(R18:R23)</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:18" ht="19" customHeight="1" x14ac:dyDescent="0.25">
@@ -1894,14 +1794,8 @@
       <c r="B25" s="22"/>
       <c r="C25" s="22"/>
       <c r="D25" s="22"/>
-      <c r="E25" s="21" t="e">
-        <f>C25/(C25+D25)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F25" s="21" t="e">
-        <f>D25/(C25+D25)</f>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="E25" s="21"/>
+      <c r="F25" s="21"/>
       <c r="G25" s="21"/>
       <c r="H25" s="8" t="s">
         <v>47</v>
@@ -1935,14 +1829,8 @@
       <c r="B26" s="22"/>
       <c r="C26" s="22"/>
       <c r="D26" s="22"/>
-      <c r="E26" s="21" t="e">
-        <f>C26/(C26+D26)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F26" s="21" t="e">
-        <f>D26/(C26+D26)</f>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="E26" s="21"/>
+      <c r="F26" s="21"/>
       <c r="G26" s="21"/>
       <c r="H26" s="21" t="s">
         <v>62</v>
@@ -1970,38 +1858,35 @@
       <c r="D27" s="22"/>
       <c r="E27" s="21"/>
       <c r="F27" s="21"/>
-      <c r="G27" s="8">
-        <f>B27</f>
-        <v>0</v>
-      </c>
+      <c r="G27" s="8"/>
       <c r="H27" s="5" t="s">
         <v>65</v>
       </c>
       <c r="K27" s="21" t="s">
         <v>66</v>
       </c>
-      <c r="L27" s="21" t="e">
+      <c r="L27" s="21">
         <f>E44</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M27" s="21" t="e">
+        <v>0</v>
+      </c>
+      <c r="M27" s="21">
         <f>F44</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N27" t="e">
+        <v>0</v>
+      </c>
+      <c r="N27">
         <f>L27</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="P27" s="21" t="s">
         <v>67</v>
       </c>
-      <c r="Q27" s="21" t="e">
+      <c r="Q27" s="21">
         <f>E46</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="R27" s="21" t="e">
+        <v>0</v>
+      </c>
+      <c r="R27" s="21">
         <f>Q27-L27</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:18" ht="19" customHeight="1" x14ac:dyDescent="0.25">
@@ -2011,14 +1896,8 @@
       <c r="B28" s="22"/>
       <c r="C28" s="22"/>
       <c r="D28" s="22"/>
-      <c r="E28" s="21" t="e">
-        <f>C28/(C28+D28)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F28" s="21" t="e">
-        <f>D28/(C28+D28)</f>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="E28" s="21"/>
+      <c r="F28" s="21"/>
       <c r="G28" s="21"/>
       <c r="H28" s="8" t="s">
         <v>68</v>
@@ -2026,28 +1905,28 @@
       <c r="K28" s="21" t="s">
         <v>62</v>
       </c>
-      <c r="L28" s="21" t="e">
+      <c r="L28" s="21">
         <f>E26</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M28" s="21" t="e">
+        <v>0</v>
+      </c>
+      <c r="M28" s="21">
         <f>F26</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N28" t="e">
+        <v>0</v>
+      </c>
+      <c r="N28">
         <f>M28</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="P28" s="21" t="s">
         <v>68</v>
       </c>
-      <c r="Q28" s="21" t="e">
+      <c r="Q28" s="21">
         <f>F28</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="R28" s="21" t="e">
+        <v>0</v>
+      </c>
+      <c r="R28" s="21">
         <f>Q28-M28</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:18" ht="19" customHeight="1" x14ac:dyDescent="0.25">
@@ -2057,14 +1936,8 @@
       <c r="B29" s="22"/>
       <c r="C29" s="22"/>
       <c r="D29" s="22"/>
-      <c r="E29" s="21" t="e">
-        <f>C29/(C29+D29)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F29" s="21" t="e">
-        <f>D29/(C29+D29)</f>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="E29" s="21"/>
+      <c r="F29" s="21"/>
       <c r="G29" s="21"/>
       <c r="H29" s="21" t="s">
         <v>38</v>
@@ -2072,28 +1945,28 @@
       <c r="K29" s="21" t="s">
         <v>69</v>
       </c>
-      <c r="L29" s="21" t="e">
+      <c r="L29" s="21">
         <f>E62</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M29" s="21" t="e">
+        <v>0</v>
+      </c>
+      <c r="M29" s="21">
         <f>F62</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N29" t="e">
+        <v>0</v>
+      </c>
+      <c r="N29">
         <f>L29</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="P29" s="21" t="s">
         <v>70</v>
       </c>
-      <c r="Q29" s="21" t="e">
+      <c r="Q29" s="21">
         <f>E64</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="R29" s="21" t="e">
+        <v>0</v>
+      </c>
+      <c r="R29" s="21">
         <f>Q29-L29</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:18" ht="19" customHeight="1" x14ac:dyDescent="0.25">
@@ -2105,38 +1978,35 @@
       <c r="D30" s="22"/>
       <c r="E30" s="21"/>
       <c r="F30" s="21"/>
-      <c r="G30" s="21">
-        <f>B30</f>
-        <v>0</v>
-      </c>
+      <c r="G30" s="21"/>
       <c r="H30" s="5" t="s">
         <v>71</v>
       </c>
       <c r="K30" s="21" t="s">
         <v>72</v>
       </c>
-      <c r="L30" s="21" t="e">
+      <c r="L30" s="21">
         <f>E35</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M30" s="21" t="e">
+        <v>0</v>
+      </c>
+      <c r="M30" s="21">
         <f>F35</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N30" t="e">
+        <v>0</v>
+      </c>
+      <c r="N30">
         <f>M30</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="P30" s="21" t="s">
         <v>73</v>
       </c>
-      <c r="Q30" s="21" t="e">
+      <c r="Q30" s="21">
         <f>F37</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="R30" s="21" t="e">
+        <v>0</v>
+      </c>
+      <c r="R30" s="21">
         <f>Q30-M30</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:18" ht="19" customHeight="1" x14ac:dyDescent="0.25">
@@ -2146,14 +2016,8 @@
       <c r="B31" s="22"/>
       <c r="C31" s="22"/>
       <c r="D31" s="22"/>
-      <c r="E31" s="21" t="e">
-        <f>C31/(C31+D31)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F31" s="21" t="e">
-        <f>D31/(C31+D31)</f>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="E31" s="21"/>
+      <c r="F31" s="21"/>
       <c r="G31" s="21"/>
       <c r="H31" s="8" t="s">
         <v>39</v>
@@ -2161,28 +2025,28 @@
       <c r="K31" s="21" t="s">
         <v>74</v>
       </c>
-      <c r="L31" s="21" t="e">
+      <c r="L31" s="21">
         <f>E68</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M31" s="21" t="e">
+        <v>0</v>
+      </c>
+      <c r="M31" s="21">
         <f>F68</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N31" t="e">
+        <v>0</v>
+      </c>
+      <c r="N31">
         <f>L31</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="P31" s="21" t="s">
         <v>75</v>
       </c>
-      <c r="Q31" s="21" t="e">
+      <c r="Q31" s="21">
         <f>E70</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="R31" s="21" t="e">
+        <v>0</v>
+      </c>
+      <c r="R31" s="21">
         <f>Q31-L31</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:18" ht="19" customHeight="1" x14ac:dyDescent="0.25">
@@ -2192,14 +2056,8 @@
       <c r="B32" s="22"/>
       <c r="C32" s="22"/>
       <c r="D32" s="22"/>
-      <c r="E32" s="21" t="e">
-        <f>C32/(C32+D32)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F32" s="21" t="e">
-        <f>D32/(C32+D32)</f>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="E32" s="21"/>
+      <c r="F32" s="21"/>
       <c r="G32" s="21"/>
       <c r="H32" s="21" t="s">
         <v>49</v>
@@ -2207,28 +2065,28 @@
       <c r="K32" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="L32" s="17" t="e">
+      <c r="L32" s="17">
         <f>AVERAGE(L26:L31)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M32" s="17" t="e">
+        <v>0</v>
+      </c>
+      <c r="M32" s="17">
         <f>AVERAGE(M26:M31)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N32" t="e">
+        <v>0</v>
+      </c>
+      <c r="N32">
         <f>AVERAGE(N26:N31)</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="P32" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="Q32" s="17" t="e">
+      <c r="Q32" s="17">
         <f>AVERAGE(Q26:Q31)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="R32" s="17" t="e">
+        <v>0</v>
+      </c>
+      <c r="R32" s="17">
         <f>AVERAGE(R26:R31)</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:18" ht="19" customHeight="1" x14ac:dyDescent="0.25">
@@ -2240,10 +2098,7 @@
       <c r="D33" s="22"/>
       <c r="E33" s="21"/>
       <c r="F33" s="21"/>
-      <c r="G33" s="21">
-        <f>B33</f>
-        <v>0</v>
-      </c>
+      <c r="G33" s="21"/>
       <c r="H33" s="5" t="s">
         <v>76</v>
       </c>
@@ -2276,14 +2131,8 @@
       <c r="B34" s="22"/>
       <c r="C34" s="22"/>
       <c r="D34" s="22"/>
-      <c r="E34" s="21" t="e">
-        <f>C34/(C34+D34)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F34" s="21" t="e">
-        <f>D34/(C34+D34)</f>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="E34" s="21"/>
+      <c r="F34" s="21"/>
       <c r="G34" s="21"/>
       <c r="H34" s="8" t="s">
         <v>50</v>
@@ -2291,28 +2140,28 @@
       <c r="K34" s="21" t="s">
         <v>79</v>
       </c>
-      <c r="L34" s="21" t="e">
+      <c r="L34" s="21">
         <f>E50</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M34" s="21" t="e">
+        <v>0</v>
+      </c>
+      <c r="M34" s="21">
         <f>F50</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N34" t="e">
+        <v>0</v>
+      </c>
+      <c r="N34">
         <f>M34</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="P34" s="21" t="s">
         <v>80</v>
       </c>
-      <c r="Q34" s="21" t="e">
+      <c r="Q34" s="21">
         <f>F52</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="R34" s="21" t="e">
+        <v>0</v>
+      </c>
+      <c r="R34" s="21">
         <f>Q34-M34</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:18" ht="19" customHeight="1" x14ac:dyDescent="0.25">
@@ -2322,14 +2171,8 @@
       <c r="B35" s="22"/>
       <c r="C35" s="22"/>
       <c r="D35" s="22"/>
-      <c r="E35" s="21" t="e">
-        <f>C35/(C35+D35)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F35" s="21" t="e">
-        <f>D35/(C35+D35)</f>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="E35" s="21"/>
+      <c r="F35" s="21"/>
       <c r="G35" s="21"/>
       <c r="H35" s="21" t="s">
         <v>72</v>
@@ -2337,28 +2180,28 @@
       <c r="K35" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="L35" s="21" t="e">
+      <c r="L35" s="21">
         <f>E14</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M35" s="21" t="e">
+        <v>0</v>
+      </c>
+      <c r="M35" s="21">
         <f>F14</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N35" t="e">
+        <v>0</v>
+      </c>
+      <c r="N35">
         <f>L35</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="P35" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="Q35" s="21" t="e">
+      <c r="Q35" s="21">
         <f>E16</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="R35" s="21" t="e">
+        <v>0</v>
+      </c>
+      <c r="R35" s="21">
         <f>Q35-L35</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:18" ht="19" customHeight="1" x14ac:dyDescent="0.25">
@@ -2370,38 +2213,35 @@
       <c r="D36" s="22"/>
       <c r="E36" s="21"/>
       <c r="F36" s="21"/>
-      <c r="G36" s="21">
-        <f>B36</f>
-        <v>0</v>
-      </c>
+      <c r="G36" s="21"/>
       <c r="H36" s="5" t="s">
         <v>81</v>
       </c>
       <c r="K36" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="L36" s="21" t="e">
+      <c r="L36" s="21">
         <f>E8</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M36" s="21" t="e">
+        <v>0</v>
+      </c>
+      <c r="M36" s="21">
         <f>F8</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N36" t="e">
+        <v>0</v>
+      </c>
+      <c r="N36">
         <f>M36</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="P36" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="Q36" s="21" t="e">
+      <c r="Q36" s="21">
         <f>F10</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="R36" s="21" t="e">
+        <v>0</v>
+      </c>
+      <c r="R36" s="21">
         <f>Q36-M36</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:18" ht="19" customHeight="1" x14ac:dyDescent="0.25">
@@ -2411,14 +2251,8 @@
       <c r="B37" s="22"/>
       <c r="C37" s="22"/>
       <c r="D37" s="22"/>
-      <c r="E37" s="21" t="e">
-        <f>C37/(C37+D37)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F37" s="21" t="e">
-        <f>D37/(C37+D37)</f>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="E37" s="21"/>
+      <c r="F37" s="21"/>
       <c r="G37" s="21"/>
       <c r="H37" s="8" t="s">
         <v>73</v>
@@ -2426,28 +2260,28 @@
       <c r="K37" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="L37" s="21" t="e">
+      <c r="L37" s="21">
         <f>E20</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M37" s="21" t="e">
+        <v>0</v>
+      </c>
+      <c r="M37" s="21">
         <f>F20</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N37" t="e">
+        <v>0</v>
+      </c>
+      <c r="N37">
         <f>L37</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="P37" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="Q37" s="21" t="e">
+      <c r="Q37" s="21">
         <f>E22</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="R37" s="21" t="e">
+        <v>0</v>
+      </c>
+      <c r="R37" s="21">
         <f>Q37-L37</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:18" ht="19" customHeight="1" x14ac:dyDescent="0.25">
@@ -2457,14 +2291,8 @@
       <c r="B38" s="22"/>
       <c r="C38" s="22"/>
       <c r="D38" s="22"/>
-      <c r="E38" s="21" t="e">
-        <f>C38/(C38+D38)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F38" s="21" t="e">
-        <f>D38/(C38+D38)</f>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="E38" s="21"/>
+      <c r="F38" s="21"/>
       <c r="G38" s="21"/>
       <c r="H38" s="21" t="s">
         <v>82</v>
@@ -2472,28 +2300,28 @@
       <c r="K38" s="21" t="s">
         <v>83</v>
       </c>
-      <c r="L38" s="21" t="e">
+      <c r="L38" s="21">
         <f>E74</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M38" s="21" t="e">
+        <v>0</v>
+      </c>
+      <c r="M38" s="21">
         <f>F74</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N38" t="e">
+        <v>0</v>
+      </c>
+      <c r="N38">
         <f>M38</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="P38" s="21" t="s">
         <v>84</v>
       </c>
-      <c r="Q38" s="21" t="e">
+      <c r="Q38" s="21">
         <f>F76</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="R38" s="21" t="e">
+        <v>0</v>
+      </c>
+      <c r="R38" s="21">
         <f>Q38-M38</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="39" spans="1:18" ht="19" customHeight="1" x14ac:dyDescent="0.25">
@@ -2505,38 +2333,35 @@
       <c r="D39" s="22"/>
       <c r="E39" s="21"/>
       <c r="F39" s="21"/>
-      <c r="G39" s="21">
-        <f>B39</f>
-        <v>0</v>
-      </c>
+      <c r="G39" s="21"/>
       <c r="H39" s="5" t="s">
         <v>85</v>
       </c>
       <c r="K39" s="21" t="s">
         <v>82</v>
       </c>
-      <c r="L39" s="21" t="e">
+      <c r="L39" s="21">
         <f>E38</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M39" s="21" t="e">
+        <v>0</v>
+      </c>
+      <c r="M39" s="21">
         <f>F38</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N39" t="e">
+        <v>0</v>
+      </c>
+      <c r="N39">
         <f>L39</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="P39" s="21" t="s">
         <v>86</v>
       </c>
-      <c r="Q39" s="21" t="e">
+      <c r="Q39" s="21">
         <f>E40</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="R39" s="21" t="e">
+        <v>0</v>
+      </c>
+      <c r="R39" s="21">
         <f>Q39-L39</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="40" spans="1:18" ht="19" customHeight="1" x14ac:dyDescent="0.25">
@@ -2546,14 +2371,8 @@
       <c r="B40" s="22"/>
       <c r="C40" s="22"/>
       <c r="D40" s="22"/>
-      <c r="E40" s="21" t="e">
-        <f>C40/(C40+D40)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F40" s="21" t="e">
-        <f>D40/(C40+D40)</f>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="E40" s="21"/>
+      <c r="F40" s="21"/>
       <c r="G40" s="21"/>
       <c r="H40" s="8" t="s">
         <v>86</v>
@@ -2561,28 +2380,28 @@
       <c r="K40" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="L40" s="17" t="e">
+      <c r="L40" s="17">
         <f>AVERAGE(L34:L39)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M40" s="17" t="e">
+        <v>0</v>
+      </c>
+      <c r="M40" s="17">
         <f>AVERAGE(M34:M39)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N40" t="e">
+        <v>0</v>
+      </c>
+      <c r="N40">
         <f>AVERAGE(N34:N39)</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="P40" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="Q40" s="17" t="e">
+      <c r="Q40" s="17">
         <f>AVERAGE(Q34:Q39)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="R40" s="17" t="e">
+        <v>0</v>
+      </c>
+      <c r="R40" s="17">
         <f>AVERAGE(R34:R39)</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:18" ht="19" customHeight="1" x14ac:dyDescent="0.25">
@@ -2592,14 +2411,8 @@
       <c r="B41" s="22"/>
       <c r="C41" s="22"/>
       <c r="D41" s="22"/>
-      <c r="E41" s="21" t="e">
-        <f>C41/(C41+D41)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F41" s="21" t="e">
-        <f>D41/(C41+D41)</f>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="E41" s="21"/>
+      <c r="F41" s="21"/>
       <c r="G41" s="21"/>
       <c r="H41" s="21" t="s">
         <v>30</v>
@@ -2607,18 +2420,18 @@
       <c r="K41" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="L41" s="27" t="s">
+      <c r="L41" s="31" t="s">
         <v>88</v>
       </c>
-      <c r="M41" s="28"/>
-      <c r="N41" s="26"/>
+      <c r="M41" s="32"/>
+      <c r="N41" s="33"/>
       <c r="P41" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="Q41" s="27" t="s">
+      <c r="Q41" s="31" t="s">
         <v>88</v>
       </c>
-      <c r="R41" s="26"/>
+      <c r="R41" s="33"/>
     </row>
     <row r="42" spans="1:18" ht="19" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="4">
@@ -2629,30 +2442,27 @@
       <c r="D42" s="22"/>
       <c r="E42" s="21"/>
       <c r="F42" s="21"/>
-      <c r="G42" s="8">
-        <f>B42</f>
-        <v>0</v>
-      </c>
+      <c r="G42" s="8"/>
       <c r="H42" s="5" t="s">
         <v>90</v>
       </c>
       <c r="K42" s="21" t="s">
         <v>91</v>
       </c>
-      <c r="L42" s="25" t="e">
+      <c r="L42" s="34">
         <f t="shared" ref="L42:L47" si="1">Q26-Q10</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M42" s="28"/>
-      <c r="N42" s="26"/>
+        <v>0</v>
+      </c>
+      <c r="M42" s="32"/>
+      <c r="N42" s="33"/>
       <c r="P42" s="21" t="s">
         <v>91</v>
       </c>
-      <c r="Q42" s="25" t="e">
+      <c r="Q42" s="34">
         <f t="shared" ref="Q42:Q47" si="2">Q34-Q18</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="R42" s="26"/>
+        <v>0</v>
+      </c>
+      <c r="R42" s="33"/>
     </row>
     <row r="43" spans="1:18" ht="19" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="4">
@@ -2661,14 +2471,8 @@
       <c r="B43" s="22"/>
       <c r="C43" s="22"/>
       <c r="D43" s="22"/>
-      <c r="E43" s="21" t="e">
-        <f>C43/(C43+D43)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F43" s="21" t="e">
-        <f>D43/(C43+D43)</f>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="E43" s="21"/>
+      <c r="F43" s="21"/>
       <c r="G43" s="21"/>
       <c r="H43" s="8" t="s">
         <v>31</v>
@@ -2676,20 +2480,20 @@
       <c r="K43" s="21" t="s">
         <v>92</v>
       </c>
-      <c r="L43" s="25" t="e">
+      <c r="L43" s="34">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M43" s="28"/>
-      <c r="N43" s="26"/>
+        <v>0</v>
+      </c>
+      <c r="M43" s="32"/>
+      <c r="N43" s="33"/>
       <c r="P43" s="21" t="s">
         <v>92</v>
       </c>
-      <c r="Q43" s="25" t="e">
+      <c r="Q43" s="34">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="R43" s="26"/>
+        <v>0</v>
+      </c>
+      <c r="R43" s="33"/>
     </row>
     <row r="44" spans="1:18" ht="19" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="4">
@@ -2698,14 +2502,8 @@
       <c r="B44" s="22"/>
       <c r="C44" s="22"/>
       <c r="D44" s="22"/>
-      <c r="E44" s="21" t="e">
-        <f>C44/(C44+D44)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F44" s="21" t="e">
-        <f>D44/(C44+D44)</f>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="E44" s="21"/>
+      <c r="F44" s="21"/>
       <c r="G44" s="21"/>
       <c r="H44" s="21" t="s">
         <v>66</v>
@@ -2713,20 +2511,20 @@
       <c r="K44" s="21" t="s">
         <v>93</v>
       </c>
-      <c r="L44" s="25" t="e">
+      <c r="L44" s="34">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M44" s="28"/>
-      <c r="N44" s="26"/>
+        <v>0</v>
+      </c>
+      <c r="M44" s="32"/>
+      <c r="N44" s="33"/>
       <c r="P44" s="21" t="s">
         <v>93</v>
       </c>
-      <c r="Q44" s="25" t="e">
+      <c r="Q44" s="34">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="R44" s="26"/>
+        <v>0</v>
+      </c>
+      <c r="R44" s="33"/>
     </row>
     <row r="45" spans="1:18" ht="19" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="4">
@@ -2737,30 +2535,27 @@
       <c r="D45" s="22"/>
       <c r="E45" s="21"/>
       <c r="F45" s="21"/>
-      <c r="G45" s="8">
-        <f>B45</f>
-        <v>0</v>
-      </c>
+      <c r="G45" s="8"/>
       <c r="H45" s="5" t="s">
         <v>94</v>
       </c>
       <c r="K45" s="21" t="s">
         <v>95</v>
       </c>
-      <c r="L45" s="25" t="e">
+      <c r="L45" s="34">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M45" s="28"/>
-      <c r="N45" s="26"/>
+        <v>0</v>
+      </c>
+      <c r="M45" s="32"/>
+      <c r="N45" s="33"/>
       <c r="P45" s="21" t="s">
         <v>95</v>
       </c>
-      <c r="Q45" s="25" t="e">
+      <c r="Q45" s="34">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="R45" s="26"/>
+        <v>0</v>
+      </c>
+      <c r="R45" s="33"/>
     </row>
     <row r="46" spans="1:18" ht="19" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="4">
@@ -2769,14 +2564,8 @@
       <c r="B46" s="22"/>
       <c r="C46" s="22"/>
       <c r="D46" s="22"/>
-      <c r="E46" s="21" t="e">
-        <f>C46/(C46+D46)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F46" s="21" t="e">
-        <f>D46/(C46+D46)</f>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="E46" s="21"/>
+      <c r="F46" s="21"/>
       <c r="G46" s="21"/>
       <c r="H46" s="8" t="s">
         <v>67</v>
@@ -2784,20 +2573,20 @@
       <c r="K46" s="21" t="s">
         <v>96</v>
       </c>
-      <c r="L46" s="25" t="e">
+      <c r="L46" s="34">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M46" s="28"/>
-      <c r="N46" s="26"/>
+        <v>0</v>
+      </c>
+      <c r="M46" s="32"/>
+      <c r="N46" s="33"/>
       <c r="P46" s="21" t="s">
         <v>96</v>
       </c>
-      <c r="Q46" s="25" t="e">
+      <c r="Q46" s="34">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="R46" s="26"/>
+        <v>0</v>
+      </c>
+      <c r="R46" s="33"/>
     </row>
     <row r="47" spans="1:18" ht="19" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="4">
@@ -2806,14 +2595,8 @@
       <c r="B47" s="22"/>
       <c r="C47" s="22"/>
       <c r="D47" s="22"/>
-      <c r="E47" s="21" t="e">
-        <f>C47/(C47+D47)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F47" s="21" t="e">
-        <f>D47/(C47+D47)</f>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="E47" s="21"/>
+      <c r="F47" s="21"/>
       <c r="G47" s="21"/>
       <c r="H47" s="21" t="s">
         <v>57</v>
@@ -2821,20 +2604,20 @@
       <c r="K47" s="21" t="s">
         <v>97</v>
       </c>
-      <c r="L47" s="25" t="e">
+      <c r="L47" s="34">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M47" s="28"/>
-      <c r="N47" s="26"/>
+        <v>0</v>
+      </c>
+      <c r="M47" s="32"/>
+      <c r="N47" s="33"/>
       <c r="P47" s="21" t="s">
         <v>97</v>
       </c>
-      <c r="Q47" s="25" t="e">
+      <c r="Q47" s="34">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="R47" s="26"/>
+        <v>0</v>
+      </c>
+      <c r="R47" s="33"/>
     </row>
     <row r="48" spans="1:18" ht="19" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="4">
@@ -2845,26 +2628,23 @@
       <c r="D48" s="22"/>
       <c r="E48" s="21"/>
       <c r="F48" s="21"/>
-      <c r="G48" s="21">
-        <f>B48</f>
-        <v>0</v>
-      </c>
+      <c r="G48" s="21"/>
       <c r="H48" s="5" t="s">
         <v>98</v>
       </c>
       <c r="L48" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="M48" s="18" t="e">
+      <c r="M48" s="18">
         <f>AVERAGE(L42:N47)</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="Q48" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="R48" s="17" t="e">
+      <c r="R48" s="17">
         <f>AVERAGE(Q42:R47)</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="49" spans="1:18" ht="19" customHeight="1" x14ac:dyDescent="0.25">
@@ -2874,14 +2654,8 @@
       <c r="B49" s="22"/>
       <c r="C49" s="22"/>
       <c r="D49" s="22"/>
-      <c r="E49" s="21" t="e">
-        <f>C49/(C49+D49)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F49" s="21" t="e">
-        <f>D49/(C49+D49)</f>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="E49" s="21"/>
+      <c r="F49" s="21"/>
       <c r="G49" s="21"/>
       <c r="H49" s="8" t="s">
         <v>58</v>
@@ -2894,31 +2668,25 @@
       <c r="B50" s="22"/>
       <c r="C50" s="22"/>
       <c r="D50" s="22"/>
-      <c r="E50" s="21" t="e">
-        <f>C50/(C50+D50)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F50" s="21" t="e">
-        <f>D50/(C50+D50)</f>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="E50" s="21"/>
+      <c r="F50" s="21"/>
       <c r="G50" s="21"/>
       <c r="H50" s="21" t="s">
         <v>79</v>
       </c>
-      <c r="J50" s="27" t="s">
+      <c r="J50" s="31" t="s">
         <v>99</v>
       </c>
-      <c r="K50" s="28"/>
-      <c r="L50" s="28"/>
-      <c r="M50" s="26"/>
+      <c r="K50" s="32"/>
+      <c r="L50" s="32"/>
+      <c r="M50" s="33"/>
       <c r="P50" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="Q50" s="27" t="s">
+      <c r="Q50" s="31" t="s">
         <v>101</v>
       </c>
-      <c r="R50" s="26"/>
+      <c r="R50" s="33"/>
     </row>
     <row r="51" spans="1:18" ht="19" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="4">
@@ -2929,14 +2697,11 @@
       <c r="D51" s="22"/>
       <c r="E51" s="21"/>
       <c r="F51" s="21"/>
-      <c r="G51" s="21">
-        <f>B51</f>
-        <v>0</v>
-      </c>
+      <c r="G51" s="21"/>
       <c r="H51" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="J51" s="31" t="s">
+      <c r="J51" s="27" t="s">
         <v>103</v>
       </c>
       <c r="K51" s="7" t="s">
@@ -2954,11 +2719,11 @@
       <c r="P51" s="21" t="s">
         <v>91</v>
       </c>
-      <c r="Q51" s="25" t="e">
+      <c r="Q51" s="34">
         <f t="shared" ref="Q51:Q56" si="3">Q34-Q26</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="R51" s="26"/>
+        <v>0</v>
+      </c>
+      <c r="R51" s="33"/>
     </row>
     <row r="52" spans="1:18" ht="19" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="4">
@@ -2967,19 +2732,13 @@
       <c r="B52" s="22"/>
       <c r="C52" s="22"/>
       <c r="D52" s="22"/>
-      <c r="E52" s="21" t="e">
-        <f>C52/(C52+D52)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F52" s="21" t="e">
-        <f>D52/(C52+D52)</f>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="E52" s="21"/>
+      <c r="F52" s="21"/>
       <c r="G52" s="21"/>
       <c r="H52" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="J52" s="32"/>
+      <c r="J52" s="28"/>
       <c r="K52" s="21" t="s">
         <v>91</v>
       </c>
@@ -2997,11 +2756,11 @@
       <c r="P52" s="21" t="s">
         <v>92</v>
       </c>
-      <c r="Q52" s="25" t="e">
+      <c r="Q52" s="34">
         <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="R52" s="26"/>
+        <v>0</v>
+      </c>
+      <c r="R52" s="33"/>
     </row>
     <row r="53" spans="1:18" ht="19" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="4">
@@ -3010,19 +2769,13 @@
       <c r="B53" s="22"/>
       <c r="C53" s="22"/>
       <c r="D53" s="22"/>
-      <c r="E53" s="21" t="e">
-        <f>C53/(C53+D53)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F53" s="21" t="e">
-        <f>D53/(C53+D53)</f>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="E53" s="21"/>
+      <c r="F53" s="21"/>
       <c r="G53" s="21"/>
       <c r="H53" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="J53" s="32"/>
+      <c r="J53" s="28"/>
       <c r="K53" s="21" t="s">
         <v>92</v>
       </c>
@@ -3041,11 +2794,11 @@
       <c r="P53" s="21" t="s">
         <v>93</v>
       </c>
-      <c r="Q53" s="25" t="e">
+      <c r="Q53" s="34">
         <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="R53" s="26"/>
+        <v>0</v>
+      </c>
+      <c r="R53" s="33"/>
     </row>
     <row r="54" spans="1:18" ht="19" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="4">
@@ -3056,14 +2809,11 @@
       <c r="D54" s="22"/>
       <c r="E54" s="21"/>
       <c r="F54" s="21"/>
-      <c r="G54" s="21">
-        <f>B54</f>
-        <v>0</v>
-      </c>
+      <c r="G54" s="21"/>
       <c r="H54" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="J54" s="32"/>
+      <c r="J54" s="28"/>
       <c r="K54" s="21" t="s">
         <v>93</v>
       </c>
@@ -3081,11 +2831,11 @@
       <c r="P54" s="21" t="s">
         <v>95</v>
       </c>
-      <c r="Q54" s="25" t="e">
+      <c r="Q54" s="34">
         <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="R54" s="26"/>
+        <v>0</v>
+      </c>
+      <c r="R54" s="33"/>
     </row>
     <row r="55" spans="1:18" ht="19" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="4">
@@ -3094,19 +2844,13 @@
       <c r="B55" s="22"/>
       <c r="C55" s="22"/>
       <c r="D55" s="22"/>
-      <c r="E55" s="21" t="e">
-        <f>C55/(C55+D55)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F55" s="21" t="e">
-        <f>D55/(C55+D55)</f>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="E55" s="21"/>
+      <c r="F55" s="21"/>
       <c r="G55" s="21"/>
       <c r="H55" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="J55" s="32"/>
+      <c r="J55" s="28"/>
       <c r="K55" s="21" t="s">
         <v>95</v>
       </c>
@@ -3125,11 +2869,11 @@
       <c r="P55" s="21" t="s">
         <v>96</v>
       </c>
-      <c r="Q55" s="25" t="e">
+      <c r="Q55" s="34">
         <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="R55" s="26"/>
+        <v>0</v>
+      </c>
+      <c r="R55" s="33"/>
     </row>
     <row r="56" spans="1:18" ht="19" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="4">
@@ -3138,19 +2882,13 @@
       <c r="B56" s="22"/>
       <c r="C56" s="22"/>
       <c r="D56" s="22"/>
-      <c r="E56" s="21" t="e">
-        <f>C56/(C56+D56)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F56" s="21" t="e">
-        <f>D56/(C56+D56)</f>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="E56" s="21"/>
+      <c r="F56" s="21"/>
       <c r="G56" s="21"/>
       <c r="H56" s="21" t="s">
         <v>63</v>
       </c>
-      <c r="J56" s="32"/>
+      <c r="J56" s="28"/>
       <c r="K56" s="21" t="s">
         <v>96</v>
       </c>
@@ -3165,11 +2903,11 @@
       <c r="P56" s="21" t="s">
         <v>97</v>
       </c>
-      <c r="Q56" s="25" t="e">
+      <c r="Q56" s="34">
         <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="R56" s="26"/>
+        <v>0</v>
+      </c>
+      <c r="R56" s="33"/>
     </row>
     <row r="57" spans="1:18" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" s="4">
@@ -3180,14 +2918,11 @@
       <c r="D57" s="22"/>
       <c r="E57" s="21"/>
       <c r="F57" s="21"/>
-      <c r="G57" s="21">
-        <f>B57</f>
-        <v>0</v>
-      </c>
+      <c r="G57" s="21"/>
       <c r="H57" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="J57" s="33"/>
+      <c r="J57" s="29"/>
       <c r="K57" s="21" t="s">
         <v>97</v>
       </c>
@@ -3202,9 +2937,9 @@
       <c r="Q57" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="R57" s="17" t="e">
+      <c r="R57" s="17">
         <f>AVERAGE(Q51:R56)</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="58" spans="1:18" ht="19" customHeight="1" x14ac:dyDescent="0.25">
@@ -3214,17 +2949,13 @@
       <c r="B58" s="22"/>
       <c r="C58" s="22"/>
       <c r="D58" s="22"/>
-      <c r="E58" s="21">
-        <v>0</v>
-      </c>
-      <c r="F58" s="21">
-        <v>0</v>
-      </c>
+      <c r="E58" s="21"/>
+      <c r="F58" s="21"/>
       <c r="G58" s="21"/>
       <c r="H58" s="21" t="s">
         <v>64</v>
       </c>
-      <c r="J58" s="34" t="s">
+      <c r="J58" s="30" t="s">
         <v>108</v>
       </c>
       <c r="K58" s="21" t="s">
@@ -3241,10 +2972,10 @@
       <c r="P58" s="7" t="s">
         <v>109</v>
       </c>
-      <c r="Q58" s="27" t="s">
+      <c r="Q58" s="31" t="s">
         <v>110</v>
       </c>
-      <c r="R58" s="26"/>
+      <c r="R58" s="33"/>
     </row>
     <row r="59" spans="1:18" ht="19" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="4">
@@ -3253,19 +2984,13 @@
       <c r="B59" s="22"/>
       <c r="C59" s="22"/>
       <c r="D59" s="22"/>
-      <c r="E59" s="21" t="e">
-        <f>C59/(C59+D59)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F59" s="21" t="e">
-        <f>D59/(C59+D59)</f>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="E59" s="21"/>
+      <c r="F59" s="21"/>
       <c r="G59" s="21"/>
       <c r="H59" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="J59" s="32"/>
+      <c r="J59" s="28"/>
       <c r="K59" s="21" t="s">
         <v>92</v>
       </c>
@@ -3283,11 +3008,11 @@
       <c r="P59" s="21" t="s">
         <v>91</v>
       </c>
-      <c r="Q59" s="25" t="e">
+      <c r="Q59" s="34">
         <f t="shared" ref="Q59:Q64" si="4">Q18-Q10</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="R59" s="26"/>
+        <v>0</v>
+      </c>
+      <c r="R59" s="33"/>
     </row>
     <row r="60" spans="1:18" ht="19" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="4">
@@ -3298,14 +3023,11 @@
       <c r="D60" s="22"/>
       <c r="E60" s="21"/>
       <c r="F60" s="21"/>
-      <c r="G60" s="21">
-        <f>B60</f>
-        <v>0</v>
-      </c>
+      <c r="G60" s="21"/>
       <c r="H60" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="J60" s="32"/>
+      <c r="J60" s="28"/>
       <c r="K60" s="21" t="s">
         <v>93</v>
       </c>
@@ -3324,11 +3046,11 @@
       <c r="P60" s="21" t="s">
         <v>92</v>
       </c>
-      <c r="Q60" s="25" t="e">
+      <c r="Q60" s="34">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="R60" s="26"/>
+        <v>0</v>
+      </c>
+      <c r="R60" s="33"/>
     </row>
     <row r="61" spans="1:18" ht="19" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="4">
@@ -3337,19 +3059,13 @@
       <c r="B61" s="22"/>
       <c r="C61" s="22"/>
       <c r="D61" s="22"/>
-      <c r="E61" s="21" t="e">
-        <f>C61/(C61+D61)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F61" s="21" t="e">
-        <f>D61/(C61+D61)</f>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="E61" s="21"/>
+      <c r="F61" s="21"/>
       <c r="G61" s="21"/>
       <c r="H61" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="J61" s="32"/>
+      <c r="J61" s="28"/>
       <c r="K61" s="21" t="s">
         <v>95</v>
       </c>
@@ -3367,11 +3083,11 @@
       <c r="P61" s="21" t="s">
         <v>93</v>
       </c>
-      <c r="Q61" s="25" t="e">
+      <c r="Q61" s="34">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="R61" s="26"/>
+        <v>0</v>
+      </c>
+      <c r="R61" s="33"/>
     </row>
     <row r="62" spans="1:18" ht="19" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="4">
@@ -3380,19 +3096,13 @@
       <c r="B62" s="22"/>
       <c r="C62" s="22"/>
       <c r="D62" s="22"/>
-      <c r="E62" s="21" t="e">
-        <f>C62/(C62+D62)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F62" s="21" t="e">
-        <f>D62/(C62+D62)</f>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="E62" s="21"/>
+      <c r="F62" s="21"/>
       <c r="G62" s="21"/>
       <c r="H62" s="21" t="s">
         <v>69</v>
       </c>
-      <c r="J62" s="32"/>
+      <c r="J62" s="28"/>
       <c r="K62" s="21" t="s">
         <v>96</v>
       </c>
@@ -3411,11 +3121,11 @@
       <c r="P62" s="21" t="s">
         <v>95</v>
       </c>
-      <c r="Q62" s="25" t="e">
+      <c r="Q62" s="34">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="R62" s="26"/>
+        <v>0</v>
+      </c>
+      <c r="R62" s="33"/>
     </row>
     <row r="63" spans="1:18" ht="19" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="4">
@@ -3426,14 +3136,11 @@
       <c r="D63" s="22"/>
       <c r="E63" s="21"/>
       <c r="F63" s="21"/>
-      <c r="G63" s="21">
-        <f>B63</f>
-        <v>0</v>
-      </c>
+      <c r="G63" s="21"/>
       <c r="H63" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="J63" s="33"/>
+      <c r="J63" s="29"/>
       <c r="K63" s="21" t="s">
         <v>97</v>
       </c>
@@ -3448,11 +3155,11 @@
       <c r="P63" s="21" t="s">
         <v>96</v>
       </c>
-      <c r="Q63" s="25" t="e">
+      <c r="Q63" s="34">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="R63" s="26"/>
+        <v>0</v>
+      </c>
+      <c r="R63" s="33"/>
     </row>
     <row r="64" spans="1:18" ht="19" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="4">
@@ -3461,14 +3168,8 @@
       <c r="B64" s="22"/>
       <c r="C64" s="22"/>
       <c r="D64" s="22"/>
-      <c r="E64" s="21" t="e">
-        <f>C64/(C64+D64)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F64" s="21" t="e">
-        <f>D64/(C64+D64)</f>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="E64" s="21"/>
+      <c r="F64" s="21"/>
       <c r="G64" s="21"/>
       <c r="H64" s="8" t="s">
         <v>70</v>
@@ -3477,11 +3178,11 @@
       <c r="P64" s="21" t="s">
         <v>97</v>
       </c>
-      <c r="Q64" s="25" t="e">
+      <c r="Q64" s="34">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="R64" s="26"/>
+        <v>0</v>
+      </c>
+      <c r="R64" s="33"/>
     </row>
     <row r="65" spans="1:18" ht="19" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="4">
@@ -3490,14 +3191,8 @@
       <c r="B65" s="22"/>
       <c r="C65" s="22"/>
       <c r="D65" s="22"/>
-      <c r="E65" s="21" t="e">
-        <f>C65/(C65+D65)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F65" s="21" t="e">
-        <f>D65/(C65+D65)</f>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="E65" s="21"/>
+      <c r="F65" s="21"/>
       <c r="G65" s="21"/>
       <c r="H65" s="21" t="s">
         <v>44</v>
@@ -3505,9 +3200,9 @@
       <c r="Q65" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="R65" s="17" t="e">
+      <c r="R65" s="17">
         <f>AVERAGE(Q59:R64)</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="66" spans="1:18" ht="19" customHeight="1" x14ac:dyDescent="0.25">
@@ -3519,10 +3214,7 @@
       <c r="D66" s="22"/>
       <c r="E66" s="21"/>
       <c r="F66" s="21"/>
-      <c r="G66" s="21">
-        <f>B66</f>
-        <v>0</v>
-      </c>
+      <c r="G66" s="21"/>
       <c r="H66" s="5" t="s">
         <v>113</v>
       </c>
@@ -3534,14 +3226,8 @@
       <c r="B67" s="22"/>
       <c r="C67" s="22"/>
       <c r="D67" s="22"/>
-      <c r="E67" s="21" t="e">
-        <f>C67/(C67+D67)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F67" s="21" t="e">
-        <f>D67/(C67+D67)</f>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="E67" s="21"/>
+      <c r="F67" s="21"/>
       <c r="G67" s="21"/>
       <c r="H67" s="8" t="s">
         <v>45</v>
@@ -3554,14 +3240,8 @@
       <c r="B68" s="22"/>
       <c r="C68" s="22"/>
       <c r="D68" s="22"/>
-      <c r="E68" s="21" t="e">
-        <f>C68/(C68+D68)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F68" s="21" t="e">
-        <f>D68/(C68+D68)</f>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="E68" s="21"/>
+      <c r="F68" s="21"/>
       <c r="G68" s="21"/>
       <c r="H68" s="21" t="s">
         <v>74</v>
@@ -3576,10 +3256,7 @@
       <c r="D69" s="22"/>
       <c r="E69" s="21"/>
       <c r="F69" s="21"/>
-      <c r="G69" s="21">
-        <f>B69</f>
-        <v>0</v>
-      </c>
+      <c r="G69" s="21"/>
       <c r="H69" s="5" t="s">
         <v>114</v>
       </c>
@@ -3591,14 +3268,8 @@
       <c r="B70" s="22"/>
       <c r="C70" s="22"/>
       <c r="D70" s="22"/>
-      <c r="E70" s="21" t="e">
-        <f>C70/(C70+D70)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F70" s="21" t="e">
-        <f>D70/(C70+D70)</f>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="E70" s="21"/>
+      <c r="F70" s="21"/>
       <c r="G70" s="21"/>
       <c r="H70" s="8" t="s">
         <v>75</v>
@@ -3611,14 +3282,8 @@
       <c r="B71" s="22"/>
       <c r="C71" s="22"/>
       <c r="D71" s="22"/>
-      <c r="E71" s="21" t="e">
-        <f>C71/(C71+D71)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F71" s="21" t="e">
-        <f>D71/(C71+D71)</f>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="E71" s="21"/>
+      <c r="F71" s="21"/>
       <c r="G71" s="21"/>
       <c r="H71" s="21" t="s">
         <v>52</v>
@@ -3633,10 +3298,7 @@
       <c r="D72" s="22"/>
       <c r="E72" s="21"/>
       <c r="F72" s="21"/>
-      <c r="G72" s="21">
-        <f>B72</f>
-        <v>0</v>
-      </c>
+      <c r="G72" s="21"/>
       <c r="H72" s="5" t="s">
         <v>115</v>
       </c>
@@ -3648,14 +3310,8 @@
       <c r="B73" s="22"/>
       <c r="C73" s="22"/>
       <c r="D73" s="22"/>
-      <c r="E73" s="21" t="e">
-        <f>C73/(C73+D73)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F73" s="21" t="e">
-        <f>D73/(C73+D73)</f>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="E73" s="21"/>
+      <c r="F73" s="21"/>
       <c r="G73" s="21"/>
       <c r="H73" s="8" t="s">
         <v>53</v>
@@ -3668,14 +3324,8 @@
       <c r="B74" s="22"/>
       <c r="C74" s="22"/>
       <c r="D74" s="22"/>
-      <c r="E74" s="21" t="e">
-        <f>C74/(C74+D74)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F74" s="21" t="e">
-        <f>D74/(C74+D74)</f>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="E74" s="21"/>
+      <c r="F74" s="21"/>
       <c r="G74" s="21"/>
       <c r="H74" s="21" t="s">
         <v>83</v>
@@ -3690,10 +3340,7 @@
       <c r="D75" s="22"/>
       <c r="E75" s="21"/>
       <c r="F75" s="21"/>
-      <c r="G75" s="21">
-        <f>B75</f>
-        <v>0</v>
-      </c>
+      <c r="G75" s="21"/>
       <c r="H75" s="5" t="s">
         <v>116</v>
       </c>
@@ -3705,14 +3352,8 @@
       <c r="B76" s="22"/>
       <c r="C76" s="22"/>
       <c r="D76" s="22"/>
-      <c r="E76" s="21" t="e">
-        <f>C76/(C76+D76)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F76" s="21" t="e">
-        <f>D76/(C76+D76)</f>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="E76" s="21"/>
+      <c r="F76" s="21"/>
       <c r="G76" s="21"/>
       <c r="H76" s="8" t="s">
         <v>84</v>
@@ -3725,14 +3366,8 @@
       <c r="B77" s="22"/>
       <c r="C77" s="22"/>
       <c r="D77" s="22"/>
-      <c r="E77" s="21" t="e">
-        <f>C77/(C77+D77)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F77" s="21" t="e">
-        <f>D77/(C77+D77)</f>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="E77" s="21"/>
+      <c r="F77" s="21"/>
       <c r="G77" s="21"/>
       <c r="H77" s="21" t="s">
         <v>27</v>
@@ -3747,10 +3382,7 @@
       <c r="D78" s="22"/>
       <c r="E78" s="21"/>
       <c r="F78" s="21"/>
-      <c r="G78" s="21">
-        <f>B78</f>
-        <v>0</v>
-      </c>
+      <c r="G78" s="21"/>
       <c r="H78" s="5" t="s">
         <v>117</v>
       </c>
@@ -3762,14 +3394,8 @@
       <c r="B79" s="22"/>
       <c r="C79" s="22"/>
       <c r="D79" s="22"/>
-      <c r="E79" s="21" t="e">
-        <f>C79/(C79+D79)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F79" s="21" t="e">
-        <f>D79/(C79+D79)</f>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="E79" s="21"/>
+      <c r="F79" s="21"/>
       <c r="G79" s="21"/>
       <c r="H79" s="21" t="s">
         <v>28</v>
@@ -3777,18 +3403,13 @@
     </row>
   </sheetData>
   <mergeCells count="32">
-    <mergeCell ref="B2:K2"/>
-    <mergeCell ref="J51:J57"/>
-    <mergeCell ref="J58:J63"/>
-    <mergeCell ref="J50:M50"/>
-    <mergeCell ref="L41:N41"/>
-    <mergeCell ref="Q41:R41"/>
-    <mergeCell ref="L42:N42"/>
-    <mergeCell ref="L43:N43"/>
-    <mergeCell ref="L44:N44"/>
-    <mergeCell ref="Q42:R42"/>
-    <mergeCell ref="Q43:R43"/>
-    <mergeCell ref="Q44:R44"/>
+    <mergeCell ref="Q63:R63"/>
+    <mergeCell ref="Q64:R64"/>
+    <mergeCell ref="Q58:R58"/>
+    <mergeCell ref="Q59:R59"/>
+    <mergeCell ref="Q60:R60"/>
+    <mergeCell ref="Q61:R61"/>
+    <mergeCell ref="Q62:R62"/>
     <mergeCell ref="Q45:R45"/>
     <mergeCell ref="Q46:R46"/>
     <mergeCell ref="Q55:R55"/>
@@ -3802,13 +3423,18 @@
     <mergeCell ref="Q52:R52"/>
     <mergeCell ref="Q53:R53"/>
     <mergeCell ref="Q54:R54"/>
-    <mergeCell ref="Q63:R63"/>
-    <mergeCell ref="Q64:R64"/>
-    <mergeCell ref="Q58:R58"/>
-    <mergeCell ref="Q59:R59"/>
-    <mergeCell ref="Q60:R60"/>
-    <mergeCell ref="Q61:R61"/>
-    <mergeCell ref="Q62:R62"/>
+    <mergeCell ref="Q41:R41"/>
+    <mergeCell ref="L42:N42"/>
+    <mergeCell ref="L43:N43"/>
+    <mergeCell ref="L44:N44"/>
+    <mergeCell ref="Q42:R42"/>
+    <mergeCell ref="Q43:R43"/>
+    <mergeCell ref="Q44:R44"/>
+    <mergeCell ref="B2:K2"/>
+    <mergeCell ref="J51:J57"/>
+    <mergeCell ref="J58:J63"/>
+    <mergeCell ref="J50:M50"/>
+    <mergeCell ref="L41:N41"/>
   </mergeCells>
   <conditionalFormatting sqref="H5:H7">
     <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">

</xml_diff>